<commit_message>
Documentation on the project "Implementation of CRM in a bank"
</commit_message>
<xml_diff>
--- a/Stakeholder Register.xlsx
+++ b/Stakeholder Register.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masha\PM\TASK\2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masha\PM\CRM_impl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="8550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11430"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="152">
   <si>
     <t>ID</t>
   </si>
@@ -82,9 +82,6 @@
     <t>mail</t>
   </si>
   <si>
-    <t>Скороденко Мария</t>
-  </si>
-  <si>
     <t>Продуктовая компания</t>
   </si>
   <si>
@@ -94,16 +91,7 @@
     <t xml:space="preserve">Руководитель проектов </t>
   </si>
   <si>
-    <t>Проэктный отдел</t>
-  </si>
-  <si>
-    <t>Винниченко Александр</t>
-  </si>
-  <si>
     <t>+380982790409</t>
-  </si>
-  <si>
-    <t>Vinnichenko@gmail.com</t>
   </si>
   <si>
     <t>telegram
@@ -121,9 +109,6 @@
     <t>Сторонник</t>
   </si>
   <si>
-    <t>Радостев Павел</t>
-  </si>
-  <si>
     <t>Член команды</t>
   </si>
   <si>
@@ -133,15 +118,9 @@
     <t>Отдел разработки</t>
   </si>
   <si>
-    <t>Трегубенко Сергей</t>
-  </si>
-  <si>
     <t>+380982790410</t>
   </si>
   <si>
-    <t>Radostev@gmail.com</t>
-  </si>
-  <si>
     <t>почта</t>
   </si>
   <si>
@@ -151,15 +130,9 @@
     <t>Формирование программно-аппаратной части сервиса.</t>
   </si>
   <si>
-    <t>Захаренко Елена</t>
-  </si>
-  <si>
     <t>+380982790411</t>
   </si>
   <si>
-    <t>Мирошниченко Марина</t>
-  </si>
-  <si>
     <t>Frontend разработчик</t>
   </si>
   <si>
@@ -169,36 +142,21 @@
     <t>Разработка пользовательского интерфейса и функций которые работают на пользовательской стороне приложения.</t>
   </si>
   <si>
-    <t>Волощук Богдан</t>
-  </si>
-  <si>
     <t>+380982790413</t>
   </si>
   <si>
-    <t>Дончук Александр</t>
-  </si>
-  <si>
     <t>Тестировщик</t>
   </si>
   <si>
     <t>Отдел тестирования</t>
   </si>
   <si>
-    <t>Карась Сергей</t>
-  </si>
-  <si>
     <t>+380982790414</t>
   </si>
   <si>
-    <t>Donchuk@gmail.com</t>
-  </si>
-  <si>
     <t>Техническое тестирование на всех этапах</t>
   </si>
   <si>
-    <t>Крученюк Сергей</t>
-  </si>
-  <si>
     <t>Банк</t>
   </si>
   <si>
@@ -208,15 +166,9 @@
     <t>Департамент корпоративного бизнеса</t>
   </si>
   <si>
-    <t>Демченко Татьяна</t>
-  </si>
-  <si>
     <t>+380982790415</t>
   </si>
   <si>
-    <t>Kruchenyuk@gmail.com</t>
-  </si>
-  <si>
     <t>Получать информацию по работе с клиентами напрямую из базы во всех разрезах деятельности. Снизить общую стоимость операций. Брендинг компании.</t>
   </si>
   <si>
@@ -229,9 +181,6 @@
     <t>принятие решения о готовности по завершению каждого этапа работ</t>
   </si>
   <si>
-    <t>Карлова Ольга</t>
-  </si>
-  <si>
     <t>Эксперт</t>
   </si>
   <si>
@@ -241,15 +190,9 @@
     <t>Отдел кадров</t>
   </si>
   <si>
-    <t>Мартынова Светлана</t>
-  </si>
-  <si>
     <t>+380982790417</t>
   </si>
   <si>
-    <t>Karlova@gmail.com</t>
-  </si>
-  <si>
     <t>Оптимизация работы сотрудников</t>
   </si>
   <si>
@@ -259,54 +202,33 @@
     <t>Нейтрал</t>
   </si>
   <si>
-    <t>Якименко Ольга</t>
-  </si>
-  <si>
     <t>Аналитик</t>
   </si>
   <si>
     <t>Отдел аналитики</t>
   </si>
   <si>
-    <t>Довнань Лилия</t>
-  </si>
-  <si>
     <t>+380982790418</t>
   </si>
   <si>
-    <t>YAkimenko@gmail.com</t>
-  </si>
-  <si>
     <t>Отвечает за описание существующий решений, формирование требований к системе. Проводит техническое тестирование.</t>
   </si>
   <si>
-    <t>Локтев Андрей</t>
-  </si>
-  <si>
     <t>ИТ архитектор</t>
   </si>
   <si>
     <t>Управление ИТ архитектуры</t>
   </si>
   <si>
-    <t>Власюк Виктория</t>
-  </si>
-  <si>
     <t>+380982790419</t>
   </si>
   <si>
-    <t>Loktev@gmail.com</t>
-  </si>
-  <si>
     <t>Отказ от разнородного програмного обезпечения. Интеграция с АБС, мобильным-банкингом</t>
   </si>
   <si>
     <t xml:space="preserve">Описание существующий решений. Участие в формировании требований к системе. </t>
   </si>
   <si>
-    <t>Довбуш Алла</t>
-  </si>
-  <si>
     <t>Эксперт/пользователь</t>
   </si>
   <si>
@@ -316,39 +238,24 @@
     <t>Отдел по работе с корпоративными клиентами</t>
   </si>
   <si>
-    <t>Татарин Валерий</t>
-  </si>
-  <si>
     <t>+380982790420</t>
   </si>
   <si>
-    <t>Dovbush@gmail.com</t>
-  </si>
-  <si>
     <t>Управление подразделением, работой менеджеров.Аналитика,планы,отчеты. Процесс передачи клиента от менеджера менеджеру менее болезнен.</t>
   </si>
   <si>
     <t>Участие в описание существующий решений. Участие в формирование требований к системе. Участие в пользовательском тестировании.</t>
   </si>
   <si>
-    <t>Иванова Ольга</t>
-  </si>
-  <si>
     <t>менеджер по продажам</t>
   </si>
   <si>
     <t>Отделение банка №1</t>
   </si>
   <si>
-    <t>Ставицкий Алексей</t>
-  </si>
-  <si>
     <t>+380982790421</t>
   </si>
   <si>
-    <t>Ivanova@gmail.com</t>
-  </si>
-  <si>
     <t>телефон</t>
   </si>
   <si>
@@ -361,45 +268,27 @@
     <t>надо провести разяснительнуя работу</t>
   </si>
   <si>
-    <t>Москвичева Анастасия</t>
-  </si>
-  <si>
     <t>Руководитель напрвления маркетинга</t>
   </si>
   <si>
     <t>Отдел маркетинга</t>
   </si>
   <si>
-    <t>Ломоносов Владислав</t>
-  </si>
-  <si>
     <t>+380982790422</t>
   </si>
   <si>
-    <t>Moskvicheva@gmail.com</t>
-  </si>
-  <si>
     <t>Автоматизация формирование списка рассылок с учетом интересов клиентов</t>
   </si>
   <si>
-    <t>Петров Сергей</t>
-  </si>
-  <si>
     <t>Руководитель направления входящей линии юридических лиц</t>
   </si>
   <si>
     <t>Контакт-центр</t>
   </si>
   <si>
-    <t>Вапняр Дмитрий</t>
-  </si>
-  <si>
     <t>+380982790423</t>
   </si>
   <si>
-    <t>Petrov@gmail.com</t>
-  </si>
-  <si>
     <t>Оперативный доступ к карточке клиента со всей нужнойинформацией</t>
   </si>
   <si>
@@ -409,84 +298,51 @@
     <t>+380982790424</t>
   </si>
   <si>
-    <t>@gmail.com</t>
-  </si>
-  <si>
-    <t>Годлис Дарья</t>
-  </si>
-  <si>
     <t>Специалист по обучению</t>
   </si>
   <si>
     <t>Отдел обучения</t>
   </si>
   <si>
-    <t>Маковей Катерина</t>
-  </si>
-  <si>
     <t>+380982790425</t>
   </si>
   <si>
-    <t>Godlis@gmail.com</t>
-  </si>
-  <si>
     <t>Интересныи опыт</t>
   </si>
   <si>
     <t>Подготовить требования для проведения обучения</t>
   </si>
   <si>
-    <t>Мельничук Людмила</t>
-  </si>
-  <si>
     <t>Сотрудник бэк-офиса</t>
   </si>
   <si>
     <t>Бэк-офис</t>
   </si>
   <si>
-    <t>Купчак Дмитрий</t>
-  </si>
-  <si>
     <t>+380982790426</t>
   </si>
   <si>
-    <t>Mel'nichuk@gmail.com</t>
-  </si>
-  <si>
     <t>Информация по сделке доступна до регистрации в АБС. Минимизация затрат со стороны бэк-офиса на верификацию сделок. Сокращение ручного вмешательства в рассчет</t>
   </si>
   <si>
     <t>Противник,боится сокращений</t>
   </si>
   <si>
-    <t>Ящук Сергей</t>
-  </si>
-  <si>
     <t>Сотрудник кредитного отдела</t>
   </si>
   <si>
     <t>Кредитный отдел</t>
   </si>
   <si>
-    <t>Турчина Анна</t>
-  </si>
-  <si>
     <t>+380982790427</t>
   </si>
   <si>
-    <t>YAschuk@gmail.com</t>
-  </si>
-  <si>
     <t>Автоматизация контроля всех видов кредитных отношений. Анализ клиента, проверка соблюдения платежей, напоминание о сроке выплат и т.д.</t>
   </si>
   <si>
     <t>сторонник</t>
   </si>
   <si>
-    <t>Мариненко Алена</t>
-  </si>
-  <si>
     <t>Пользователь</t>
   </si>
   <si>
@@ -496,9 +352,6 @@
     <t>+380982790428</t>
   </si>
   <si>
-    <t>Marinenko@gmail.com</t>
-  </si>
-  <si>
     <t>Быстрый, удобный доступ к предложениям банка. Наличие чатадля оперативной связи с контактцентром.</t>
   </si>
   <si>
@@ -524,6 +377,120 @@
   </si>
   <si>
     <t>Спонсор</t>
+  </si>
+  <si>
+    <t>Проектный отдел</t>
+  </si>
+  <si>
+    <t>SH#1</t>
+  </si>
+  <si>
+    <t>SH#2</t>
+  </si>
+  <si>
+    <t>SH#3</t>
+  </si>
+  <si>
+    <t>SH#4</t>
+  </si>
+  <si>
+    <t>SH#5</t>
+  </si>
+  <si>
+    <t>SH#6</t>
+  </si>
+  <si>
+    <t>SH#7</t>
+  </si>
+  <si>
+    <t>SH#8</t>
+  </si>
+  <si>
+    <t>SH#9</t>
+  </si>
+  <si>
+    <t>SH#10</t>
+  </si>
+  <si>
+    <t>SH#11</t>
+  </si>
+  <si>
+    <t>SH#12</t>
+  </si>
+  <si>
+    <t>SH#13</t>
+  </si>
+  <si>
+    <t>SH#14</t>
+  </si>
+  <si>
+    <t>SH#15</t>
+  </si>
+  <si>
+    <t>SH#16</t>
+  </si>
+  <si>
+    <t>SH#17</t>
+  </si>
+  <si>
+    <t>SH#18</t>
+  </si>
+  <si>
+    <t>SH#19</t>
+  </si>
+  <si>
+    <t>SH#20</t>
+  </si>
+  <si>
+    <t>SH#21</t>
+  </si>
+  <si>
+    <t>SH#22</t>
+  </si>
+  <si>
+    <t>SH#23</t>
+  </si>
+  <si>
+    <t>SH#24</t>
+  </si>
+  <si>
+    <t>SH#25</t>
+  </si>
+  <si>
+    <t>SH#26</t>
+  </si>
+  <si>
+    <t>SH#27</t>
+  </si>
+  <si>
+    <t>SH#28</t>
+  </si>
+  <si>
+    <t>SH#29</t>
+  </si>
+  <si>
+    <t>SH#30</t>
+  </si>
+  <si>
+    <t>SH#31</t>
+  </si>
+  <si>
+    <t>SH#32</t>
+  </si>
+  <si>
+    <t>SH#33</t>
+  </si>
+  <si>
+    <t>SH#34</t>
+  </si>
+  <si>
+    <t>SH#35</t>
+  </si>
+  <si>
+    <t>SH#36</t>
+  </si>
+  <si>
+    <t>SH#37</t>
   </si>
 </sst>
 </file>
@@ -661,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -714,15 +681,18 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1007,7 +977,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1042,8 +1012,8 @@
       <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
-        <v>158</v>
+      <c r="E1" s="24" t="s">
+        <v>109</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>4</v>
@@ -1054,10 +1024,10 @@
       <c r="H1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="25"/>
+      <c r="J1" s="26"/>
       <c r="K1" s="22" t="s">
         <v>8</v>
       </c>
@@ -1104,46 +1074,47 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="J3" s="15" t="str">
+        <f>CONCATENATE(B3,"@gmail.com")</f>
+        <v>SH#1@gmail.com</v>
+      </c>
+      <c r="K3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="L3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>26</v>
       </c>
       <c r="N3" s="15">
         <v>8</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P3" s="16"/>
     </row>
@@ -1152,46 +1123,47 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="15" t="str">
+        <f t="shared" ref="J4:J22" si="0">CONCATENATE(B4,"@gmail.com")</f>
+        <v>SH#2@gmail.com</v>
+      </c>
+      <c r="K4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="L4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F4" s="15" t="s">
+      <c r="M4" s="16" t="s">
         <v>30</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>37</v>
       </c>
       <c r="N4" s="15">
         <v>6</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P4" s="16"/>
     </row>
@@ -1200,46 +1172,47 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#3@gmail.com</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="F5" s="15" t="s">
+      <c r="M5" s="16" t="s">
         <v>30</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>37</v>
       </c>
       <c r="N5" s="15">
         <v>6</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P5" s="16"/>
     </row>
@@ -1248,46 +1221,47 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#4@gmail.com</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="15" t="s">
+      <c r="M6" s="16" t="s">
         <v>34</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>43</v>
       </c>
       <c r="N6" s="15">
         <v>5</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P6" s="16"/>
     </row>
@@ -1296,46 +1270,47 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#5@gmail.com</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="15" t="s">
+      <c r="M7" s="16" t="s">
         <v>34</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>43</v>
       </c>
       <c r="N7" s="15">
         <v>5</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P7" s="16"/>
     </row>
@@ -1344,46 +1319,47 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#6@gmail.com</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>36</v>
-      </c>
       <c r="M8" s="16" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="N8" s="15">
         <v>4</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P8" s="16"/>
     </row>
@@ -1392,73 +1368,81 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>159</v>
+        <v>110</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="J9" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#7@gmail.com</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="N9" s="2">
         <v>6</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" s="11" customFormat="1" ht="28.5">
-      <c r="A10" s="2">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>122</v>
+      </c>
       <c r="C10" s="8" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="5" t="s">
-        <v>35</v>
+      <c r="H10" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#8@gmail.com</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="M10" s="9"/>
       <c r="N10" s="8"/>
@@ -1470,46 +1454,47 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>70</v>
+        <v>51</v>
+      </c>
+      <c r="J11" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#9@gmail.com</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="N11" s="2">
         <v>3</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="P11" s="3"/>
     </row>
@@ -1518,46 +1503,47 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>77</v>
+        <v>141</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>79</v>
+        <v>57</v>
+      </c>
+      <c r="J12" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#10@gmail.com</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="N12" s="2">
         <v>8</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P12" s="3"/>
     </row>
@@ -1566,46 +1552,47 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>86</v>
+        <v>61</v>
+      </c>
+      <c r="J13" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#11@gmail.com</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="N13" s="2">
         <v>7</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P13" s="3"/>
     </row>
@@ -1614,46 +1601,47 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>95</v>
+        <v>67</v>
+      </c>
+      <c r="J14" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#12@gmail.com</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="N14" s="2">
         <v>7</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P14" s="3"/>
     </row>
@@ -1662,49 +1650,50 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>103</v>
+        <v>72</v>
+      </c>
+      <c r="J15" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#13@gmail.com</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="N15" s="2">
         <v>5</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="57">
@@ -1712,46 +1701,47 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>113</v>
+        <v>79</v>
+      </c>
+      <c r="J16" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#14@gmail.com</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="N16" s="2">
         <v>5</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P16" s="3"/>
     </row>
@@ -1760,46 +1750,47 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>120</v>
+        <v>83</v>
+      </c>
+      <c r="J17" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#15@gmail.com</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="N17" s="2">
         <v>4</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P17" s="3"/>
     </row>
@@ -1807,24 +1798,29 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="C18" s="8" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="8"/>
+      <c r="H18" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="I18" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>124</v>
+        <v>86</v>
+      </c>
+      <c r="J18" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#16@gmail.com</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="10"/>
@@ -1838,46 +1834,47 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>130</v>
+        <v>89</v>
+      </c>
+      <c r="J19" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#17@gmail.com</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="N19" s="2">
         <v>5</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="P19" s="3"/>
     </row>
@@ -1886,49 +1883,50 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>138</v>
+        <v>94</v>
+      </c>
+      <c r="J20" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#18@gmail.com</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="N20" s="2">
         <v>5</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="71.25">
@@ -1936,46 +1934,47 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>146</v>
+        <v>99</v>
+      </c>
+      <c r="J21" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#19@gmail.com</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="N21" s="2">
         <v>5</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="P21" s="3"/>
     </row>
@@ -1984,40 +1983,43 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="2"/>
       <c r="I22" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>153</v>
+        <v>104</v>
+      </c>
+      <c r="J22" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>SH#20@gmail.com</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="N22" s="2">
         <v>5</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P22" s="3"/>
     </row>
@@ -2026,13 +2028,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:F2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="H1:H2"/>
@@ -2041,6 +2036,13 @@
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>